<commit_message>
The connection and database processes are implemented with JPA and Hibernate, the security of the application is implemented with spring security in the config package
</commit_message>
<xml_diff>
--- a/src/main/resources/static/InitialGymData.xlsx
+++ b/src/main/resources/static/InitialGymData.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GymFinalProject\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE9600F-4DCC-4D41-AA2F-8023F6AF09DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{414D6F96-D5BC-442B-B4B5-A9333F309541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6C74A0C4-BBDA-4BE1-BA5A-893169BA97A5}"/>
   </bookViews>
   <sheets>
-    <sheet name="User" sheetId="4" r:id="rId1"/>
-    <sheet name="Trainee" sheetId="1" r:id="rId2"/>
-    <sheet name="Training_Type" sheetId="5" r:id="rId3"/>
-    <sheet name="Trainer" sheetId="2" r:id="rId4"/>
-    <sheet name="Training" sheetId="3" r:id="rId5"/>
+    <sheet name="Trainee" sheetId="1" r:id="rId1"/>
+    <sheet name="Training_Type" sheetId="5" r:id="rId2"/>
+    <sheet name="Trainer" sheetId="2" r:id="rId3"/>
+    <sheet name="Training" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
   <si>
     <t>Id</t>
   </si>
@@ -477,97 +476,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3EA9408-A494-4768-8892-129CC3F2E88A}">
-  <dimension ref="A1:F4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82179A81-FDB9-4596-84E9-A62702528452}">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="4" max="4" width="19.26953125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="H2" s="5">
+        <v>38205</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
+      <c r="H3" s="5">
+        <v>38052</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -575,77 +581,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82179A81-FDB9-4596-84E9-A62702528452}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="5">
-        <v>38205</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" s="5">
-        <v>38052</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="5">
-        <v>38113</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE91E5AD-29A1-45EA-9E4E-FAFA073633D8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -680,20 +615,22 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA722FC2-3315-412F-A8EF-9D4BD41AD712}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="15.26953125" customWidth="1"/>
+    <col min="7" max="7" width="14.90625" customWidth="1"/>
+    <col min="8" max="8" width="15.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -701,17 +638,47 @@
         <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2">
         <v>1</v>
       </c>
     </row>
@@ -720,12 +687,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04C02824-EEC3-4CEF-9D82-681C17B92F01}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -763,7 +730,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>

</xml_diff>